<commit_message>
Enhance contract and invoice handling with botanical name integration
- Added optional botanicalName field to contract specification schema for improved product identification.
- Updated invoice retrieval logic to include contract specifications, enhancing the generation of FSS Excel documents.
- Implemented a function to extract botanical names from contract specifications based on product names, improving accuracy in generated outputs.
- Refactored Excel generation logic to utilize botanical names, ensuring clarity and consistency in the final documents.
- Enhanced UI in the Invoices component to reflect branch-specific row coloring for better visual distinction.
</commit_message>
<xml_diff>
--- a/backend/templates/FSS_template.xlsx
+++ b/backend/templates/FSS_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11870\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6033ED-73B0-4D00-B576-42AE537FF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E623B56-31F3-4641-BE46-D8B6354AB4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,7 +633,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -656,10 +656,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -970,14 +979,14 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="73.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="38.42578125" style="6" customWidth="1"/>
@@ -1034,10 +1043,10 @@
       <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1050,7 +1059,7 @@
     <row r="2" spans="1:16" customFormat="1" ht="15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,8 +1081,8 @@
       <c r="L2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -1084,7 +1093,7 @@
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>

</xml_diff>